<commit_message>
ExcelReaderUtility modified now can handles value of any datatype using DataFormatter class
</commit_message>
<xml_diff>
--- a/src/main/java/com/test_data/Testdata.xlsx
+++ b/src/main/java/com/test_data/Testdata.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{84E5EEE2-B5BE-4FEA-8FE0-5B5B0625E823}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prate\workspace\DataDrivenUsingTestNG\src\main\java\com\test_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F667BD-1434-4E18-A162-417ECFBFFCA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="20790" windowHeight="11820" activeTab="1" xr2:uid="{AA9F958B-5541-4697-98E8-76E4CA607973}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19770" windowHeight="11760" activeTab="1" xr2:uid="{AA9F958B-5541-4697-98E8-76E4CA607973}"/>
   </bookViews>
   <sheets>
     <sheet name="FreeCrmData" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,6 @@
     <sheet name="FbLoginData" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>FirstName</t>
   </si>
@@ -162,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -331,6 +335,21 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -349,7 +368,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -364,40 +383,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -830,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44E435B4-F545-434D-AF3A-FDBD44952FDE}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,83 +837,83 @@
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="15">
+        <v>123</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="15">
+        <v>456</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="15">
+        <v>789</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="15">
+        <v>123</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="15">
+        <v>345</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -934,6 +926,7 @@
     <hyperlink ref="C6" r:id="rId5" xr:uid="{71BA344A-714D-4725-ABB4-3669FA20B3B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>